<commit_message>
Added a new homework
</commit_message>
<xml_diff>
--- a/MirelaCvetkova/Lesson8/BUGS1.xlsx
+++ b/MirelaCvetkova/Lesson8/BUGS1.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
     <sheet name="&quot;My store&quot;" sheetId="1" r:id="rId1"/>
     <sheet name="https   phptravels.com " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -78,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="50">
   <si>
     <t>Priority</t>
   </si>
@@ -189,17 +190,142 @@
     <t>Localization not applied everywhere.</t>
   </si>
   <si>
-    <t>1.Open https://phptravels.com/
+    <t>P2</t>
+  </si>
+  <si>
+    <t>03.11.2018</t>
+  </si>
+  <si>
+    <t>B04</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>When change the language from English to Estonian, many of the fields remain in English</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open https://phptravels.com/
 2.Click "Login" button
-3.Click "Account"and in dropdown list press "Register" 
-4.Enter only spaces in "Password" field. 
- Actual result:
-А green progress bar appears under the "Password" field
-Expected result:
-When enter "Space" don't appears green progress bar.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Open https://phptravels.com/
+3.Enter Email: mira1929@abv.bg
+4.Enter Password: 123412
+5.Click "Login" button
+6.Choose Estonian language in the field top right
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The fields as "Your Info","Your Active Products/Services" and " Recent Support Tickets" are English
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When change language to Estonian all texts should be in Estonian</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Login </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open https://phptravels.com/
+2.Click "Login" button
+3.Enter Email: mira1929@abv.bg
+4.Enter Password: 123412
+5.Click "Login" button
+6.Choose Italian language in the field top right
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+The fields as "Your Info","Your Active Products/Services" and " Recent Support Tickets" are English
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When change language to Italian all texts should be in Italian</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open https://phptravels.com/
 2.Click "Login" button
 3.Enter Email: mira1929@abv.bg
 4.Enter Password: 123412
@@ -207,47 +333,281 @@
 6.Click "Login"button
 7.Click "Logout" button and "You have been successfully logged out. Click here to continue" a message appears.
 8.Click "Click here to continue" 
-Actual result:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 "Login page" with empty fields appears.
-Expected result:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 After Click "Remember me" check box the data are saved for future inputs.
 </t>
-  </si>
-  <si>
-    <t>1.Open https://phptravels.com/
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open https://phptravels.com/
+2.Click "Login" button
+3.Click "Account"and in dropdown list press "Register" 
+4.Enter only spaces in "Password" field. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+А green progress bar appears under the "Password" field
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When enter "Space" don't appears green progress bar.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open http://automationpractice.com/index.php 
+2.Click "Sign in" button. 
+3.Enter email address: mira1929@abv.bg and click "Create an account" button 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+In field "Country" there is only "USA" as an option in dropdown list. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ In dropdown list should be Bulgaria as  an option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open http://automationpractice.com/index.php 
+2.Click "Sale 70% off all products"  at the top. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ There isn't result. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Expected result: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+After clicks "Sale 70% off all products" shows clothes with 70% discount.</t>
+    </r>
+  </si>
+  <si>
+    <t>When change the language from English to Hrvatski, many of the fields remain in English</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1.Open https://phptravels.com/
 2.Click "Login" button
 3.Enter Email: mira1929@abv.bg
 4.Enter Password: 123412
 5.Click "Login" button
-6.Choose Italian language in the field top right
-Actual result:
+6.Choose Hrvatski language in the field top right
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actual result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 The fields as "Your Info","Your Active Products/Services" and " Recent Support Tickets" are English
-Expected result:
-When change language to Italian all texts should be in Italian</t>
-  </si>
-  <si>
-    <t>1.Open http://automationpractice.com/index.php 
-2.Click "Sale 70% off all products"  at the top. 
-Actual result:
- There isn't result. 
-Expected result: 
-After clicks "Sale 70% off all products" shows clothes with 70% discount.</t>
-  </si>
-  <si>
-    <t>1.Open http://automationpractice.com/index.php 
-2.Click "Sign in" button. 
-3.Enter email address: mira1929@abv.bg and click "Create an account" button 
-Actual result:
-In field "Country" there is only "USA" as an option in dropdown list. 
-Expected result:
- In dropdown list should be Bulgaria as  an option</t>
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Expected result:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+When change language to Hrvatski all texts should be in Hrvatski</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +650,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -504,7 +879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -550,6 +925,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -841,6 +1226,77 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2114550</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4362450</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4827270" y="28575"/>
+          <a:ext cx="2247900" cy="516255"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2114550</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2247900" cy="516255"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4827270" y="20038695"/>
+          <a:ext cx="2247900" cy="516255"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1133,8 +1589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1146,18 +1602,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="18"/>
+      <c r="B1" s="24"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1200,16 +1656,16 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>40</v>
+      <c r="B9" s="25" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="26"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
@@ -1282,18 +1738,18 @@
     </row>
     <row r="23" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="18"/>
+      <c r="B24" s="24"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
@@ -1336,16 +1792,16 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B32" s="19" t="s">
-        <v>39</v>
+      <c r="B32" s="25" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
-      <c r="B33" s="20"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="26"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
@@ -1431,8 +1887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,18 +1898,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="32"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
@@ -1500,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -1595,18 +2051,18 @@
       <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="34"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="36"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="31"/>
-      <c r="B28" s="32"/>
+      <c r="A28" s="37"/>
+      <c r="B28" s="38"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
@@ -1653,7 +2109,7 @@
         <v>7</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1735,18 +2191,18 @@
       <c r="B47" s="4"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="28"/>
+      <c r="B48" s="34"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="29"/>
-      <c r="B49" s="30"/>
+      <c r="A49" s="35"/>
+      <c r="B49" s="36"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="31"/>
-      <c r="B50" s="32"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="38"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="11" t="s">
@@ -1793,7 +2249,7 @@
         <v>7</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="194.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1866,22 +2322,269 @@
       <c r="A67" s="9"/>
       <c r="B67" s="10"/>
     </row>
-    <row r="68" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="B68" s="4"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="4"/>
-      <c r="B69" s="4"/>
-    </row>
-    <row r="88" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A69" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B69" s="30"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="31"/>
+      <c r="B70" s="32"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="31"/>
+      <c r="B71" s="32"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78" s="18"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" s="18"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B81" s="14"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B83" s="18"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B86" s="22"/>
+    </row>
+    <row r="88" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="30"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" s="31"/>
+      <c r="B91" s="32"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="31"/>
+      <c r="B92" s="32"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="151.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" s="18"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B100" s="18"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="14"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="18"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B105" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" s="22"/>
+    </row>
+    <row r="109" spans="1:2" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="130" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
+    <mergeCell ref="A90:B92"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="A48:B50"/>
     <mergeCell ref="A26:B28"/>
+    <mergeCell ref="A69:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>